<commit_message>
update one new generation data.
</commit_message>
<xml_diff>
--- a/Pacman/Pacman/Databackup/Pacman.xlsx
+++ b/Pacman/Pacman/Databackup/Pacman.xlsx
@@ -45,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +53,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,17 +91,187 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -91,6 +282,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:E18" totalsRowShown="0" headerRowDxfId="0" dataDxfId="2" headerRowBorderDxfId="1">
+  <autoFilter ref="A1:E18"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Generation" dataDxfId="7"/>
+    <tableColumn id="2" name="Max Average Points" dataDxfId="6"/>
+    <tableColumn id="3" name="Min Average Points" dataDxfId="5"/>
+    <tableColumn id="4" name="Max points of the first Pacman" dataDxfId="4"/>
+    <tableColumn id="5" name="Count positive number of the first Pacman" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,294 +595,772 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>-72</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>-324</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>30</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>-59</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>-264</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>-62</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>-285</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>-59</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>-241</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>-55</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>-225</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>-64</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>-202</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>20</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-50</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>-219</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-44</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>-210</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>20</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-41</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>-233</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-50</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>-205</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>20</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>-32</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>-161</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>20</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>-25</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>-179</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>20</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>-43</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>-182</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>20</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>-21</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>-150</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>20</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>-27</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>-160</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>20</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>24</v>
       </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>-29</v>
+      </c>
+      <c r="C17" s="3">
+        <v>-153</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="4"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="4"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="4"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="4"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="4"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>